<commit_message>
updating milestone as well
</commit_message>
<xml_diff>
--- a/Q3/time_log.xlsx
+++ b/Q3/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_Part1\Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B61576F-DCC8-4EE5-BB9D-9AD25C20C14B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03236B34-21CA-45EB-96B6-358C5E3B2ECF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3255" yWindow="1650" windowWidth="16755" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1123,9 +1123,11 @@
         <v>43567</v>
       </c>
       <c r="D8" s="15">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="F8" s="15"/>
+        <v>0.79791666666666661</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.81805555555555554</v>
+      </c>
       <c r="H8" t="s">
         <v>47</v>
       </c>
@@ -1134,9 +1136,15 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="C9" s="14">
+        <v>43567</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.81805555555555554</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0.85138888888888886</v>
+      </c>
       <c r="H9" t="s">
         <v>43</v>
       </c>
@@ -1145,9 +1153,15 @@
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="C10" s="14">
+        <v>43567</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.90138888888888891</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0.95000000000000007</v>
+      </c>
       <c r="H10" t="s">
         <v>44</v>
       </c>
@@ -1156,9 +1170,15 @@
       <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="C11" s="14">
+        <v>43567</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.95624999999999993</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.97986111111111107</v>
+      </c>
       <c r="H11" t="s">
         <v>46</v>
       </c>
@@ -1167,9 +1187,15 @@
       <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="C12" s="14">
+        <v>43567</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.97986111111111107</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="H12" t="s">
         <v>49</v>
       </c>

</xml_diff>